<commit_message>
Regeln für pervertierung und Seele angepasst.
</commit_message>
<xml_diff>
--- a/input/books/Regelwerke/Grundregeln/Seele/KorumptionDaten.xlsx
+++ b/input/books/Regelwerke/Grundregeln/Seele/KorumptionDaten.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patri\source\repos\nota\input\books\Regelwerke\Grundregeln\Seele\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71EE6CA-1799-4D17-A880-44F3C2DD4111}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328CDAC6-09FD-42FB-899C-B7812881D62A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="7620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Daten" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
-  <si>
-    <t>Resistenz</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Normal</t>
   </si>
@@ -46,22 +43,46 @@
     <t>Miasma</t>
   </si>
   <si>
-    <t>Anstekungs wahrscheinlichket</t>
-  </si>
-  <si>
-    <t>Anfällig</t>
-  </si>
-  <si>
-    <t>Modifier</t>
-  </si>
-  <si>
     <t>Einfluss</t>
   </si>
   <si>
-    <t>Multipier</t>
-  </si>
-  <si>
-    <t>Wert</t>
+    <t>Resistent II</t>
+  </si>
+  <si>
+    <t>Resistent I</t>
+  </si>
+  <si>
+    <t>Einfluss^2</t>
+  </si>
+  <si>
+    <t>Korruption</t>
+  </si>
+  <si>
+    <t>Korruption^2</t>
+  </si>
+  <si>
+    <t>Einfluss Koruption</t>
+  </si>
+  <si>
+    <t>Const</t>
+  </si>
+  <si>
+    <t>Einfluss Quadrat</t>
+  </si>
+  <si>
+    <t>Koruption Quadrat</t>
+  </si>
+  <si>
+    <t>Einflus ^2 Koruption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einfluss Kuruptiom^2 </t>
+  </si>
+  <si>
+    <t>Anfällig I</t>
+  </si>
+  <si>
+    <t>Anfällig II</t>
   </si>
 </sst>
 </file>
@@ -105,16 +126,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -128,24 +154,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{964C339F-6FDB-4E45-8D83-5BA3D86D5162}" name="MiasmaWahrscheinlichkeit" displayName="MiasmaWahrscheinlichkeit" ref="C6:D9" totalsRowShown="0">
-  <autoFilter ref="C6:D9" xr:uid="{095980D8-5917-4D1A-8F4D-E2AF1A76B2F9}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{964C339F-6FDB-4E45-8D83-5BA3D86D5162}" name="MiasmaWahrscheinlichkeit" displayName="MiasmaWahrscheinlichkeit" ref="C6:M11" totalsRowShown="0" headerRowCellStyle="Standard">
+  <autoFilter ref="C6:M11" xr:uid="{095980D8-5917-4D1A-8F4D-E2AF1A76B2F9}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{634D5DB4-2A61-4C32-9F05-E6D113D9B430}" name="Miasma"/>
-    <tableColumn id="2" xr3:uid="{2A190532-72A8-491D-AD12-C29FB6E60CA9}" name="Anstekungs wahrscheinlichket" dataCellStyle="Prozent"/>
+    <tableColumn id="2" xr3:uid="{2A190532-72A8-491D-AD12-C29FB6E60CA9}" name="Einfluss^2" dataDxfId="0" dataCellStyle="Prozent"/>
+    <tableColumn id="3" xr3:uid="{86F002B0-AA59-407D-8D39-A4A2B3715F26}" name="Einfluss"/>
+    <tableColumn id="4" xr3:uid="{73B06010-8ED0-44F3-88B0-639E4A22A34E}" name="Korruption^2"/>
+    <tableColumn id="5" xr3:uid="{4D98414C-986F-44B9-BE6F-78BE25AA0E72}" name="Korruption"/>
+    <tableColumn id="6" xr3:uid="{DFE27731-94BB-489A-BF04-06A05FABC012}" name="Einfluss Koruption"/>
+    <tableColumn id="7" xr3:uid="{D6DF29F8-2B3F-481B-95E7-4FE129D31831}" name="Const"/>
+    <tableColumn id="8" xr3:uid="{A2BF94DC-1CF6-44F7-BBE8-E6161A208A12}" name="Einfluss Quadrat"/>
+    <tableColumn id="9" xr3:uid="{95F40862-C5E4-4CB4-9400-E79B4171D58D}" name="Koruption Quadrat"/>
+    <tableColumn id="10" xr3:uid="{52B284DD-938E-49FC-B787-AC7597AC1E34}" name="Einflus ^2 Koruption"/>
+    <tableColumn id="11" xr3:uid="{017697D8-89BC-44AA-96DD-675E77BA4E80}" name="Einfluss Kuruptiom^2 "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2589F54B-1247-411A-9BB8-81C7F03419D1}" name="Tabelle2" displayName="Tabelle2" ref="F6:G8" totalsRowShown="0">
-  <autoFilter ref="F6:G8" xr:uid="{65044614-91EC-47A7-A500-411CCBCA7D97}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F1A21109-CB2C-4D60-88E6-59BC5ECE6296}" name="Modifier"/>
-    <tableColumn id="2" xr3:uid="{6A63FDB2-3777-445D-9257-F8458A1CB9FC}" name="Wert"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -446,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="C6:G22"/>
+  <dimension ref="C6:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,85 +482,238 @@
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="F6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>6</v>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>-0.7</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="3:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>100</v>
+      </c>
+      <c r="J7">
+        <v>0.5</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>100</v>
+      </c>
+      <c r="J8">
+        <v>0.5</v>
+      </c>
+      <c r="K8">
         <v>1</v>
       </c>
-      <c r="D8" s="2">
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>-1.8</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>100</v>
+      </c>
+      <c r="J9">
         <v>0.5</v>
       </c>
-      <c r="F8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="3:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="10" spans="3:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="3:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="3:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>-3</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>15</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>100</v>
+      </c>
+      <c r="J10">
+        <v>0.5</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>-4</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>15</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>100</v>
+      </c>
+      <c r="J11">
+        <v>0.5</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="3:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="3:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="3:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="3:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="3:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="3:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="3:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="3:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="D16" s="2"/>
     </row>
     <row r="17" spans="3:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
@@ -558,16 +735,11 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="3:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="1">
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>